<commit_message>
Better analysis of units & cases
</commit_message>
<xml_diff>
--- a/Data/Events over TIme.xlsx
+++ b/Data/Events over TIme.xlsx
@@ -16,12 +16,10 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet2!$A$2:$A$87</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet2!$C$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet2!$C$2:$C$87</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet2!$B$1:$E$87</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -6078,8 +6076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="O46" sqref="O46"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7483,11 +7481,42 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D2:E86">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{47F7500B-0376-484A-A087-1C5F022D8D27}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{47F7500B-0376-484A-A087-1C5F022D8D27}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D2:E86</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>